<commit_message>
Simplify Excel Notes configuration by removing worksheet dependencies
- Remove WorksheetConfiguration class and worksheet-based Excel access
- Refactor ExcelReaderService to access tables directly across all worksheets
- Update configuration to use only table names (SHEET_INDEX, EXCEL_NOTES, {series}_NOTES)
- Improve sheet naming examples to cover all supported formats (1-3 letters, 1-3 digits)
- Update UI components to display table names instead of worksheet names
- Maintain backward compatibility while simplifying configuration structure

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/testdata/ProjectIndex.xlsx
+++ b/testdata/ProjectIndex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevorp\Dev\KPFF.AutoCAD.DraftingAssistant\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB6FD4C-BD9A-490F-8C3A-0DE981B4346C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B1BE15-8686-4093-8866-F7BFE8291200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="3690" windowWidth="38640" windowHeight="21120" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
+    <workbookView xWindow="-23148" yWindow="9684" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Sheet</t>
   </si>
@@ -46,27 +46,12 @@
     <t>Title</t>
   </si>
   <si>
-    <t>PV-101</t>
-  </si>
-  <si>
-    <t>PV-102</t>
-  </si>
-  <si>
-    <t>PAVING PLAN</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
     <t>Note</t>
   </si>
   <si>
-    <t>NOTE 1</t>
-  </si>
-  <si>
-    <t>NOTE 2</t>
-  </si>
-  <si>
     <t>Note 1</t>
   </si>
   <si>
@@ -149,6 +134,15 @@
   </si>
   <si>
     <t>PROJ-ABC-100</t>
+  </si>
+  <si>
+    <t>ABC PLAN</t>
+  </si>
+  <si>
+    <t>CONSTRUCT CURB</t>
+  </si>
+  <si>
+    <t>CONSTRUCT SIDEWALK</t>
   </si>
 </sst>
 </file>
@@ -611,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A56E6E1-F0E6-45B8-A4FD-BDCEFA26A2B5}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -627,7 +621,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -635,24 +629,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -667,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A58DC59-E790-4B42-8F44-52FF796EA0AA}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -677,10 +671,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -688,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -696,7 +690,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -711,7 +705,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF1246F-34C5-4C20-93A7-4C83B8F18203}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -723,81 +719,81 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
         <v>24</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
         <v>25</v>
       </c>
-      <c r="S1" t="s">
+      <c r="X1" t="s">
         <v>26</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>27</v>
-      </c>
-      <c r="U1" t="s">
-        <v>28</v>
-      </c>
-      <c r="V1" t="s">
-        <v>29</v>
-      </c>
-      <c r="W1" t="s">
-        <v>30</v>
-      </c>
-      <c r="X1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -808,7 +804,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>1</v>

</xml_diff>

<commit_message>
Simplify Excel reader and enhance palette manager functionality
- Streamline ExcelReaderService by removing worksheet-specific configurations
- Add ConstructionNote model for better data encapsulation
- Enhance AutoCadPaletteManager with improved command registration and error handling
- Update project configurations for better debugging experience
- Remove obsolete worksheet lookup logic in favor of direct table access

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/testdata/ProjectIndex.xlsx
+++ b/testdata/ProjectIndex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevorp\Dev\KPFF.AutoCAD.DraftingAssistant\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B1BE15-8686-4093-8866-F7BFE8291200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B92702-A802-444C-A253-F823E70C0C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="9684" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
+    <workbookView xWindow="-22956" yWindow="9816" windowWidth="23016" windowHeight="13656" activeTab="2" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -661,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A58DC59-E790-4B42-8F44-52FF796EA0AA}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -705,9 +705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF1246F-34C5-4C20-93A7-4C83B8F18203}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -798,9 +796,6 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Fix service provider build timing to resolve KPFF command execution
- Remove automatic service provider building from constructor and first access
- Implement explicit two-phase service registration (basic → full → build)
- Fix command execution to use direct logger before services are initialized
- Eliminate "Cannot register services after the service provider has been built" error
- Ensure KPFF command properly initializes services and shows palette
- Remove AutoCAD lock files from test data

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/testdata/ProjectIndex.xlsx
+++ b/testdata/ProjectIndex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevorp\Dev\KPFF.AutoCAD.DraftingAssistant\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B92702-A802-444C-A253-F823E70C0C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA44405-1004-4A38-9E6D-5FFDF4287DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22956" yWindow="9816" windowWidth="23016" windowHeight="13656" activeTab="2" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -705,7 +705,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF1246F-34C5-4C20-93A7-4C83B8F18203}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Add automatic ProjectWise initialization fix on plugin load
- Add Application.Idle event handler to automatically trigger ESC after plugin loads
- Implement ProjectWiseFix class that sends ESC characters to trigger ProjectWise ODMA loading
- Fix crashes caused by ProjectWise integration when opening drawings
- Use SendStringToExecute with ESC character (\x1B) for reliable key simulation
- Include comprehensive timestamped logging for debugging and verification
- Add robust error handling to prevent AutoCAD startup disruption

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/testdata/ProjectIndex.xlsx
+++ b/testdata/ProjectIndex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevorp\Dev\KPFF.AutoCAD.DraftingAssistant\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA44405-1004-4A38-9E6D-5FFDF4287DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B1BE15-8686-4093-8866-F7BFE8291200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
+    <workbookView xWindow="-23148" yWindow="9684" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -661,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A58DC59-E790-4B42-8F44-52FF796EA0AA}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -705,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF1246F-34C5-4C20-93A7-4C83B8F18203}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -798,6 +798,9 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Implement Phase 3 Excel integration with ClosedXML
- Add ClosedXML 0.104.0 NuGet package for Excel file reading
- Create ExcelReaderService with async processing and error handling
- Extract SheetNoteMapping class to separate file for better organization
- Implement comprehensive table reading (SHEET_INDEX, {SERIES}_NOTES, EXCEL_NOTES)
- Add data validation with column limits and duplicate consolidation
- Replace PlaceholderExcelReader with real implementation in DI container
- Update CLAUDE.md with Excel integration architecture documentation
- Verify functionality with TestConsole and real Excel test data

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/testdata/ProjectIndex.xlsx
+++ b/testdata/ProjectIndex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevorp\Dev\KPFF.AutoCAD.DraftingAssistant\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B1BE15-8686-4093-8866-F7BFE8291200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7F0D2B-98A7-4049-A0BF-03480B63404C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="9684" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
+    <workbookView xWindow="-23148" yWindow="9684" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -661,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A58DC59-E790-4B42-8F44-52FF796EA0AA}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -705,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF1246F-34C5-4C20-93A7-4C83B8F18203}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -798,9 +798,6 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Fix construction note block assignment to use sequential NT blocks
Previously, the system incorrectly mapped note numbers directly to block names:
- Note 3 → NT03 (would fail if NT03 doesn't exist)
- Note 4 → NT04 (would fail if NT04 doesn't exist)

Now uses sequential assignment based on position in list:
- First note (regardless of number) → NT01
- Second note (regardless of number) → NT02
- etc.

This ensures notes [3,4] on a sheet go to NT01 and NT02 blocks,
matching the expected behavior where construction note blocks
are filled sequentially regardless of the note numbers.

Key changes:
- ExternalDrawingManager: Changed from noteEntry.NoteNumber to (i + 1) for targetBlockName
- Added detailed logging showing "sequential assignment: position X"
- All test scenarios (ABC-103, DEF-103) now work correctly
- 100% success rate on TESTPRODUCTIONBATCH with 6 sheets processed

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/testdata/ProjectIndex.xlsx
+++ b/testdata/ProjectIndex.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevorp\Dev\KPFF.AutoCAD.DraftingAssistant\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7F0D2B-98A7-4049-A0BF-03480B63404C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CA3CD2-C153-42FF-966E-D3BCF4C80EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="9684" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9912" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
     <sheet name="ABC Notes" sheetId="2" r:id="rId2"/>
-    <sheet name="Excel Notes" sheetId="4" r:id="rId3"/>
+    <sheet name="DEF Notes" sheetId="5" r:id="rId3"/>
+    <sheet name="Excel Notes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Sheet</t>
   </si>
@@ -143,6 +144,42 @@
   </si>
   <si>
     <t>CONSTRUCT SIDEWALK</t>
+  </si>
+  <si>
+    <t>ABC-103</t>
+  </si>
+  <si>
+    <t>CONSTRUCT ROADWAY</t>
+  </si>
+  <si>
+    <t>CONSTRUCT UTILITY</t>
+  </si>
+  <si>
+    <t>GIVE SOMEONE A HIGH FIVE</t>
+  </si>
+  <si>
+    <t>BE NICE</t>
+  </si>
+  <si>
+    <t>PICK UP TRASH</t>
+  </si>
+  <si>
+    <t>EAT HEALTHY</t>
+  </si>
+  <si>
+    <t>DEF-101</t>
+  </si>
+  <si>
+    <t>DEF-102</t>
+  </si>
+  <si>
+    <t>DEF-103</t>
+  </si>
+  <si>
+    <t>DEF PLAN</t>
+  </si>
+  <si>
+    <t>PROJ-DEF-100</t>
   </si>
 </sst>
 </file>
@@ -204,8 +241,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}" name="SHEET_INDEX" displayName="SHEET_INDEX" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}" name="SHEET_INDEX" displayName="SHEET_INDEX" ref="A1:C7" totalsRowShown="0">
+  <autoFilter ref="A1:C7" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{78A15FFA-B285-4FDD-B8E2-3A938FDC2100}" name="Sheet"/>
     <tableColumn id="3" xr3:uid="{3F2713EA-FF09-4ABE-994F-102E702E9565}" name="File"/>
@@ -216,8 +253,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}" name="ABC_NOTES" displayName="ABC_NOTES" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}" name="ABC_NOTES" displayName="ABC_NOTES" ref="A1:B5" totalsRowShown="0">
+  <autoFilter ref="A1:B5" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1DFF5014-936E-44DB-A95A-177B5B5D0D2C}" name="Number"/>
     <tableColumn id="2" xr3:uid="{17C40AE7-34F1-444F-8AA3-0E51BE46689D}" name="Note"/>
@@ -227,8 +264,19 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C167B881-E5F9-44DB-8BC8-EC4D2F202D87}" name="EXCEL_NOTES" displayName="EXCEL_NOTES" ref="A1:Y3" totalsRowShown="0">
-  <autoFilter ref="A1:Y3" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A184BDBD-A5F9-44CB-A083-C6BD71A9816B}" name="DEF_NOTES" displayName="DEF_NOTES" ref="A1:B5" totalsRowShown="0">
+  <autoFilter ref="A1:B5" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{05061837-533E-4FDE-B2B4-0C0FEBE640B0}" name="Number"/>
+    <tableColumn id="2" xr3:uid="{F88F5096-9448-4440-90B8-70315526FE26}" name="Note"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C167B881-E5F9-44DB-8BC8-EC4D2F202D87}" name="EXCEL_NOTES" displayName="EXCEL_NOTES" ref="A1:Y7" totalsRowShown="0">
+  <autoFilter ref="A1:Y7" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -603,50 +651,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A56E6E1-F0E6-45B8-A4FD-BDCEFA26A2B5}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A58DC59-E790-4B42-8F44-52FF796EA0AA}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="20.6328125" customWidth="1"/>
-    <col min="3" max="3" width="50.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
       <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -657,19 +812,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A58DC59-E790-4B42-8F44-52FF796EA0AA}">
-  <dimension ref="A1:B3"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE7284E-F66F-4B31-BB75-3E5641C2CCDF}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="50.6328125" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -677,20 +834,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -701,20 +874,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF1246F-34C5-4C20-93A7-4C83B8F18203}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="25" width="10.6328125" customWidth="1"/>
+    <col min="1" max="25" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -791,23 +964,70 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C5">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement multi-style Auto Notes and series selection UI enhancements
- Enhanced MultileaderAnalyzer to support multiple multileader styles with backward compatibility
- Updated AutoNotesService to use MultileaderStyleNames list for comprehensive style filtering
- Added Project Configuration Window with dark-themed UI for editing project settings
- Implemented Series Selection Dialog for bulk sheet selection by drawing series
- Enhanced Sheet Selection Dialog with Select Series button for improved UX
- Updated project configuration model to support list-based multileader styles
- Added DarkGroupBoxStyle to theme for consistent UI appearance
- Maintained backward compatibility through legacy property support

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/testdata/ProjectIndex.xlsx
+++ b/testdata/ProjectIndex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevorp\Dev\KPFF.AutoCAD.DraftingAssistant\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CA3CD2-C153-42FF-966E-D3BCF4C80EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDB12E1-A9B8-40F3-93E4-D067D64DC8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9912" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="23256" windowHeight="13896" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -164,9 +164,6 @@
     <t>PICK UP TRASH</t>
   </si>
   <si>
-    <t>EAT HEALTHY</t>
-  </si>
-  <si>
     <t>DEF-101</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>PROJ-DEF-100</t>
+  </si>
+  <si>
+    <t>HI HENRY</t>
   </si>
 </sst>
 </file>
@@ -654,7 +654,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,35 +710,35 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -755,7 +755,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,7 +817,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,7 +863,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -879,7 +879,7 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -999,7 +999,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>3</v>

</xml_diff>

<commit_message>
Fix lock violations in dynamic block insertion with proper document locking
- Move default config path to DBRT Test project location
- Add configurable file paths for construction note blocks (NTXX.dwg) and title blocks
- Update Project Configuration UI with NTXX File Location and Title Blocks tab
- Implement proper AutoCAD 2025 document locking pattern for Database.Insert operations
- Resolve eLockViolation errors by wrapping entire block insertion process in DocumentLock
- Support dynamic blocks with preserved attributes and properties
- Remove hardcoded fallback paths, require configuration for flexibility

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/testdata/ProjectIndex.xlsx
+++ b/testdata/ProjectIndex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevorp\Dev\KPFF.AutoCAD.DraftingAssistant\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDB12E1-A9B8-40F3-93E4-D067D64DC8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453CAD98-11C0-48D0-8CDE-92FCBBED44CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="23256" windowHeight="13896" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
+    <workbookView xWindow="-23148" yWindow="9684" windowWidth="23256" windowHeight="13896" xr2:uid="{123DF31C-48EF-4A6A-B8F8-E91D0D74B0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>Sheet</t>
   </si>
@@ -137,49 +137,70 @@
     <t>PROJ-ABC-100</t>
   </si>
   <si>
+    <t>CONSTRUCT CURB</t>
+  </si>
+  <si>
+    <t>CONSTRUCT SIDEWALK</t>
+  </si>
+  <si>
+    <t>ABC-103</t>
+  </si>
+  <si>
+    <t>CONSTRUCT ROADWAY</t>
+  </si>
+  <si>
+    <t>CONSTRUCT UTILITY</t>
+  </si>
+  <si>
+    <t>DEF-101</t>
+  </si>
+  <si>
+    <t>DEF-102</t>
+  </si>
+  <si>
+    <t>DEF-103</t>
+  </si>
+  <si>
+    <t>PROJ-DEF-100</t>
+  </si>
+  <si>
+    <t>Designed By</t>
+  </si>
+  <si>
+    <t>Checked By</t>
+  </si>
+  <si>
+    <t>Approved By</t>
+  </si>
+  <si>
+    <t>TMP</t>
+  </si>
+  <si>
+    <t>ALP</t>
+  </si>
+  <si>
+    <t>CBP</t>
+  </si>
+  <si>
+    <t>FROM EXCEL</t>
+  </si>
+  <si>
+    <t>CONSTRUCT</t>
+  </si>
+  <si>
+    <t>INSTALL</t>
+  </si>
+  <si>
+    <t>PROTECT</t>
+  </si>
+  <si>
+    <t>ADJUST</t>
+  </si>
+  <si>
     <t>ABC PLAN</t>
   </si>
   <si>
-    <t>CONSTRUCT CURB</t>
-  </si>
-  <si>
-    <t>CONSTRUCT SIDEWALK</t>
-  </si>
-  <si>
-    <t>ABC-103</t>
-  </si>
-  <si>
-    <t>CONSTRUCT ROADWAY</t>
-  </si>
-  <si>
-    <t>CONSTRUCT UTILITY</t>
-  </si>
-  <si>
-    <t>GIVE SOMEONE A HIGH FIVE</t>
-  </si>
-  <si>
-    <t>BE NICE</t>
-  </si>
-  <si>
-    <t>PICK UP TRASH</t>
-  </si>
-  <si>
-    <t>DEF-101</t>
-  </si>
-  <si>
-    <t>DEF-102</t>
-  </si>
-  <si>
-    <t>DEF-103</t>
-  </si>
-  <si>
     <t>DEF PLAN</t>
-  </si>
-  <si>
-    <t>PROJ-DEF-100</t>
-  </si>
-  <si>
-    <t>HI HENRY</t>
   </si>
 </sst>
 </file>
@@ -201,15 +222,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -217,17 +244,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -241,20 +337,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}" name="SHEET_INDEX" displayName="SHEET_INDEX" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{78A15FFA-B285-4FDD-B8E2-3A938FDC2100}" name="Sheet"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}" name="SHEET_INDEX" displayName="SHEET_INDEX" ref="A1:F7" totalsRowShown="0">
+  <autoFilter ref="A1:F7" xr:uid="{A4F1CBB4-2842-41F7-ABFB-5882B559A8DC}"/>
+  <tableColumns count="6">
     <tableColumn id="3" xr3:uid="{3F2713EA-FF09-4ABE-994F-102E702E9565}" name="File"/>
+    <tableColumn id="4" xr3:uid="{491846AA-90A1-489B-8390-792C5C135E7F}" name="Sheet"/>
     <tableColumn id="2" xr3:uid="{7D6B8106-6BE9-42B2-9860-2FA6BA96E661}" name="Title"/>
+    <tableColumn id="5" xr3:uid="{0E4A50F3-5C36-48E6-8740-12D9CE401BBB}" name="Designed By" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4DB85713-0457-4BE5-A410-FCE80123A20C}" name="Checked By" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{E5E36AF6-F67D-4B8D-997A-B74EBA5B6B71}" name="Approved By" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}" name="ABC_NOTES" displayName="ABC_NOTES" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}" name="ABC_NOTES" displayName="ABC_NOTES" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1DFF5014-936E-44DB-A95A-177B5B5D0D2C}" name="Number"/>
     <tableColumn id="2" xr3:uid="{17C40AE7-34F1-444F-8AA3-0E51BE46689D}" name="Note"/>
@@ -264,8 +363,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A184BDBD-A5F9-44CB-A083-C6BD71A9816B}" name="DEF_NOTES" displayName="DEF_NOTES" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A184BDBD-A5F9-44CB-A083-C6BD71A9816B}" name="DEF_NOTES" displayName="DEF_NOTES" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{E359F877-B40D-42DD-AD11-884AE097F861}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{05061837-533E-4FDE-B2B4-0C0FEBE640B0}" name="Number"/>
     <tableColumn id="2" xr3:uid="{F88F5096-9448-4440-90B8-70315526FE26}" name="Note"/>
@@ -651,93 +750,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A56E6E1-F0E6-45B8-A4FD-BDCEFA26A2B5}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="50.6640625" customWidth="1"/>
+    <col min="1" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="3" width="50.6328125" customWidth="1"/>
+    <col min="4" max="6" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -752,19 +912,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A58DC59-E790-4B42-8F44-52FF796EA0AA}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="50.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="50.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -772,36 +930,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -814,19 +980,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE7284E-F66F-4B31-BB75-3E5641C2CCDF}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="50.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="50.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -834,36 +1000,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -879,15 +1053,15 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="25" width="10.6640625" customWidth="1"/>
+    <col min="1" max="25" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -964,70 +1138,52 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>